<commit_message>
enviamos el excel de la segunda parte
</commit_message>
<xml_diff>
--- a/IIT-25-05/PARTE II/CLASE/Ejercicios Integradores Tema 08.xlsx
+++ b/IIT-25-05/PARTE II/CLASE/Ejercicios Integradores Tema 08.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANETH LUANA\Desktop\CIBERTEC-2015\CIBERTEC-2015\SEMANA11\IIT\PARTE II\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="701"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="701" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="1" r:id="rId1"/>
@@ -36,9 +31,11 @@
     <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'01'!$C$6:$C$103</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'02'!$G$6:$G$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'01'!$B$6:$J$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'02'!$B$6:$J$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'03'!$B$6:$J$103</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'04'!$A$7:$F$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'05'!$B$6:$J$103</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'06'!$A$6:$F$97</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'08'!$B$6:$J$103</definedName>
     <definedName name="_TAB1998">[1]Cuadro_52!#REF!</definedName>
@@ -53,6 +50,7 @@
     <definedName name="IEric04">[2]IE_04!$C$2:$AM$82</definedName>
     <definedName name="jj">#REF!</definedName>
     <definedName name="jj___0">#REF!</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="TAB1998___0">#REF!</definedName>
     <definedName name="TAB1998___16">[4]Cuadro_52!#REF!</definedName>
     <definedName name="TAB1998___22">[5]Cuadro_52!#REF!</definedName>
@@ -4987,7 +4985,6 @@
     <cellStyle name="Cálculo" xfId="20" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="21" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="22" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="39" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="23" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="24" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="25" builtinId="33" customBuiltin="1"/>
@@ -5008,11 +5005,12 @@
     <cellStyle name="Texto de advertencia" xfId="36" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="37" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="38" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="39" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="40" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="41" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5021,8 +5019,35 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="1"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5781,7 +5806,7 @@
             <a:t>no empi</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-419" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="x-none" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000080"/>
               </a:solidFill>
@@ -6769,7 +6794,7 @@
             <a:t>Tome en cuenta que los resultados deberán verse a partir de la columna  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-419" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="x-none" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000080"/>
               </a:solidFill>
@@ -25736,7 +25761,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -25771,7 +25796,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -25980,13 +26005,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="B2:J103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26048,7 +26073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -26077,7 +26102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -26106,7 +26131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -26135,7 +26160,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -26164,7 +26189,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -26193,7 +26218,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
@@ -26280,7 +26305,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
@@ -26309,7 +26334,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
@@ -26338,7 +26363,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
@@ -26396,7 +26421,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
@@ -26454,7 +26479,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>80</v>
       </c>
@@ -26483,7 +26508,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
@@ -26541,7 +26566,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>55</v>
       </c>
@@ -26570,7 +26595,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
@@ -26599,7 +26624,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
@@ -26628,7 +26653,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
@@ -26657,7 +26682,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>110</v>
       </c>
@@ -26686,7 +26711,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>110</v>
       </c>
@@ -26715,7 +26740,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>110</v>
       </c>
@@ -26744,7 +26769,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>123</v>
       </c>
@@ -26773,7 +26798,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>129</v>
       </c>
@@ -26802,7 +26827,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>134</v>
       </c>
@@ -26831,7 +26856,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>139</v>
       </c>
@@ -26860,7 +26885,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>144</v>
       </c>
@@ -26889,7 +26914,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>149</v>
       </c>
@@ -26918,7 +26943,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>154</v>
       </c>
@@ -26947,7 +26972,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>159</v>
       </c>
@@ -26976,7 +27001,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>123</v>
       </c>
@@ -27005,7 +27030,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>139</v>
       </c>
@@ -27034,7 +27059,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>159</v>
       </c>
@@ -27063,7 +27088,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>178</v>
       </c>
@@ -27092,7 +27117,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>183</v>
       </c>
@@ -27121,7 +27146,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>188</v>
       </c>
@@ -27150,7 +27175,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>193</v>
       </c>
@@ -27179,7 +27204,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>198</v>
       </c>
@@ -27208,7 +27233,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>203</v>
       </c>
@@ -27237,7 +27262,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>208</v>
       </c>
@@ -27266,7 +27291,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>213</v>
       </c>
@@ -27295,7 +27320,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>219</v>
       </c>
@@ -27324,7 +27349,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>224</v>
       </c>
@@ -27353,7 +27378,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>224</v>
       </c>
@@ -27382,7 +27407,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>208</v>
       </c>
@@ -27411,7 +27436,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>237</v>
       </c>
@@ -27440,7 +27465,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>242</v>
       </c>
@@ -27469,7 +27494,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>242</v>
       </c>
@@ -27498,7 +27523,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>251</v>
       </c>
@@ -27527,7 +27552,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>256</v>
       </c>
@@ -27556,7 +27581,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>256</v>
       </c>
@@ -27585,7 +27610,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>265</v>
       </c>
@@ -27614,7 +27639,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>271</v>
       </c>
@@ -27643,7 +27668,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>276</v>
       </c>
@@ -27672,7 +27697,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>281</v>
       </c>
@@ -27701,7 +27726,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>286</v>
       </c>
@@ -27730,7 +27755,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>291</v>
       </c>
@@ -27759,7 +27784,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>296</v>
       </c>
@@ -27788,7 +27813,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>301</v>
       </c>
@@ -27817,7 +27842,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>306</v>
       </c>
@@ -27846,7 +27871,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>311</v>
       </c>
@@ -27875,7 +27900,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>311</v>
       </c>
@@ -27904,7 +27929,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>321</v>
       </c>
@@ -27933,7 +27958,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>326</v>
       </c>
@@ -27962,7 +27987,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>331</v>
       </c>
@@ -27991,7 +28016,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>331</v>
       </c>
@@ -28020,7 +28045,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>340</v>
       </c>
@@ -28049,7 +28074,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>345</v>
       </c>
@@ -28078,7 +28103,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>321</v>
       </c>
@@ -28107,7 +28132,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>355</v>
       </c>
@@ -28136,7 +28161,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>360</v>
       </c>
@@ -28165,7 +28190,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>355</v>
       </c>
@@ -28194,7 +28219,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>360</v>
       </c>
@@ -28223,7 +28248,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>355</v>
       </c>
@@ -28252,7 +28277,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>376</v>
       </c>
@@ -28281,7 +28306,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>381</v>
       </c>
@@ -28310,7 +28335,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>331</v>
       </c>
@@ -28339,7 +28364,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>389</v>
       </c>
@@ -28368,7 +28393,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>394</v>
       </c>
@@ -28397,7 +28422,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>400</v>
       </c>
@@ -28426,7 +28451,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>404</v>
       </c>
@@ -28455,7 +28480,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>409</v>
       </c>
@@ -28484,7 +28509,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>414</v>
       </c>
@@ -28513,7 +28538,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>418</v>
       </c>
@@ -28542,7 +28567,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>422</v>
       </c>
@@ -28571,7 +28596,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>426</v>
       </c>
@@ -28600,7 +28625,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>432</v>
       </c>
@@ -28629,7 +28654,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>437</v>
       </c>
@@ -28658,7 +28683,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>432</v>
       </c>
@@ -28687,7 +28712,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>446</v>
       </c>
@@ -28716,7 +28741,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>451</v>
       </c>
@@ -28745,7 +28770,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>451</v>
       </c>
@@ -28774,7 +28799,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>460</v>
       </c>
@@ -28803,7 +28828,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>465</v>
       </c>
@@ -28832,7 +28857,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>470</v>
       </c>
@@ -28862,6 +28887,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B6:J103">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Moreno Gallardo"/>
+        <filter val="Mori"/>
+        <filter val="Moscoso"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J61" r:id="rId1" display="mailto:Pestrada@uni.edu.pe"/>
@@ -30715,12 +30749,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="B2:J103"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30810,7 +30846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -30839,7 +30875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -30897,7 +30933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -30926,7 +30962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
@@ -30955,7 +30991,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
@@ -30984,7 +31020,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -31042,7 +31078,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
@@ -31071,7 +31107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
@@ -31129,7 +31165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
@@ -31158,7 +31194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
@@ -31187,7 +31223,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>80</v>
       </c>
@@ -31216,7 +31252,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
@@ -31274,7 +31310,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>55</v>
       </c>
@@ -31332,7 +31368,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
@@ -31361,7 +31397,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
@@ -31390,7 +31426,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>110</v>
       </c>
@@ -31419,7 +31455,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>110</v>
       </c>
@@ -31448,7 +31484,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>110</v>
       </c>
@@ -31535,7 +31571,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>134</v>
       </c>
@@ -31564,7 +31600,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>139</v>
       </c>
@@ -31593,7 +31629,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>144</v>
       </c>
@@ -31651,7 +31687,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>154</v>
       </c>
@@ -31680,7 +31716,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>159</v>
       </c>
@@ -31709,7 +31745,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>123</v>
       </c>
@@ -31738,7 +31774,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>139</v>
       </c>
@@ -31767,7 +31803,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>159</v>
       </c>
@@ -31825,7 +31861,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>183</v>
       </c>
@@ -31912,7 +31948,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>198</v>
       </c>
@@ -31999,7 +32035,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>213</v>
       </c>
@@ -32028,7 +32064,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>219</v>
       </c>
@@ -32173,7 +32209,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>242</v>
       </c>
@@ -32231,7 +32267,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>251</v>
       </c>
@@ -32260,7 +32296,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>256</v>
       </c>
@@ -32289,7 +32325,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>256</v>
       </c>
@@ -32376,7 +32412,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>276</v>
       </c>
@@ -32463,7 +32499,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>291</v>
       </c>
@@ -32492,7 +32528,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>296</v>
       </c>
@@ -32608,7 +32644,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>311</v>
       </c>
@@ -32637,7 +32673,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>321</v>
       </c>
@@ -32666,7 +32702,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>326</v>
       </c>
@@ -32753,7 +32789,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>475</v>
       </c>
@@ -32840,7 +32876,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>355</v>
       </c>
@@ -32898,7 +32934,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>355</v>
       </c>
@@ -32927,7 +32963,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>360</v>
       </c>
@@ -32956,7 +32992,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>355</v>
       </c>
@@ -32985,7 +33021,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>376</v>
       </c>
@@ -33014,7 +33050,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>381</v>
       </c>
@@ -33043,7 +33079,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>331</v>
       </c>
@@ -33072,7 +33108,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>389</v>
       </c>
@@ -33130,7 +33166,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>400</v>
       </c>
@@ -33159,7 +33195,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>404</v>
       </c>
@@ -33188,7 +33224,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>476</v>
       </c>
@@ -33217,7 +33253,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>414</v>
       </c>
@@ -33275,7 +33311,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>422</v>
       </c>
@@ -33333,7 +33369,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>432</v>
       </c>
@@ -33362,7 +33398,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>437</v>
       </c>
@@ -33391,7 +33427,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>432</v>
       </c>
@@ -33420,7 +33456,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>446</v>
       </c>
@@ -33449,7 +33485,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>451</v>
       </c>
@@ -33507,7 +33543,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>460</v>
       </c>
@@ -33536,7 +33572,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>465</v>
       </c>
@@ -33565,7 +33601,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>470</v>
       </c>
@@ -33595,6 +33631,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B6:J103">
+    <filterColumn colId="3">
+      <customFilters and="1">
+        <customFilter operator="greaterThanOrEqual" val="1000"/>
+        <customFilter operator="lessThanOrEqual" val="1500"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J61" r:id="rId1" display="mailto:Pestrada@uni.edu.pe"/>
@@ -33613,13 +33657,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="B2:J103"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33739,7 +33783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -33797,7 +33841,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -33855,7 +33899,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
@@ -33884,7 +33928,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -33913,7 +33957,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
@@ -33942,7 +33986,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
@@ -33971,7 +34015,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
@@ -34000,7 +34044,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
@@ -34029,7 +34073,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
@@ -34058,7 +34102,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
@@ -34087,7 +34131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>80</v>
       </c>
@@ -34116,7 +34160,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
@@ -34145,7 +34189,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>90</v>
       </c>
@@ -34174,7 +34218,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>55</v>
       </c>
@@ -34203,7 +34247,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
@@ -34232,7 +34276,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
@@ -34261,7 +34305,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
@@ -34290,7 +34334,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>110</v>
       </c>
@@ -34319,7 +34363,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>110</v>
       </c>
@@ -34348,7 +34392,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>110</v>
       </c>
@@ -34464,7 +34508,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>139</v>
       </c>
@@ -34493,7 +34537,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>144</v>
       </c>
@@ -34551,7 +34595,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>154</v>
       </c>
@@ -34638,7 +34682,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>139</v>
       </c>
@@ -34725,7 +34769,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>183</v>
       </c>
@@ -34899,7 +34943,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>213</v>
       </c>
@@ -34928,7 +34972,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>219</v>
       </c>
@@ -35160,7 +35204,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>256</v>
       </c>
@@ -35363,7 +35407,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>291</v>
       </c>
@@ -35653,7 +35697,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>475</v>
       </c>
@@ -35798,7 +35842,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>355</v>
       </c>
@@ -35827,7 +35871,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>360</v>
       </c>
@@ -35856,7 +35900,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>355</v>
       </c>
@@ -35943,7 +35987,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="16" t="s">
         <v>331</v>
       </c>
@@ -36030,7 +36074,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>400</v>
       </c>
@@ -36088,7 +36132,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>476</v>
       </c>
@@ -36233,7 +36277,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>432</v>
       </c>
@@ -36407,7 +36451,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>460</v>
       </c>
@@ -36465,7 +36509,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>470</v>
       </c>
@@ -36495,6 +36539,27 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B6:J103">
+    <filterColumn colId="3">
+      <customFilters and="1">
+        <customFilter operator="greaterThanOrEqual" val="1000"/>
+        <customFilter operator="lessThanOrEqual" val="2000"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Ate - Vitarte"/>
+        <filter val="Chorrillos"/>
+        <filter val="Jesús María"/>
+        <filter val="La Molina"/>
+        <filter val="Lima"/>
+        <filter val="Los Olivos"/>
+        <filter val="San Borja"/>
+        <filter val="San Miguel"/>
+        <filter val="Surco"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="J61" r:id="rId1" display="mailto:Pestrada@uni.edu.pe"/>
     <hyperlink ref="J67" r:id="rId2" display="mailto:galarcon63@hotmail.com"/>
@@ -36512,13 +36577,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A7:F99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -36553,7 +36618,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>1349</v>
       </c>
@@ -36573,7 +36638,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>1345</v>
       </c>
@@ -36593,7 +36658,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>1341</v>
       </c>
@@ -36613,7 +36678,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>1337</v>
       </c>
@@ -36633,7 +36698,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>1333</v>
       </c>
@@ -36653,7 +36718,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>1329</v>
       </c>
@@ -36673,7 +36738,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>1325</v>
       </c>
@@ -36693,7 +36758,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>1321</v>
       </c>
@@ -36713,7 +36778,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>1317</v>
       </c>
@@ -36733,7 +36798,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>1313</v>
       </c>
@@ -36753,7 +36818,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>1309</v>
       </c>
@@ -36773,7 +36838,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>1305</v>
       </c>
@@ -36793,7 +36858,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>1301</v>
       </c>
@@ -36813,7 +36878,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>1297</v>
       </c>
@@ -36833,7 +36898,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>1293</v>
       </c>
@@ -36853,7 +36918,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>1289</v>
       </c>
@@ -36873,7 +36938,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>1285</v>
       </c>
@@ -36893,7 +36958,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>1280</v>
       </c>
@@ -36933,7 +36998,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>1272</v>
       </c>
@@ -36973,7 +37038,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>1264</v>
       </c>
@@ -36993,7 +37058,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>1260</v>
       </c>
@@ -37013,7 +37078,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>1256</v>
       </c>
@@ -37033,7 +37098,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>1251</v>
       </c>
@@ -37053,7 +37118,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>1247</v>
       </c>
@@ -37073,7 +37138,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>1243</v>
       </c>
@@ -37093,7 +37158,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>1239</v>
       </c>
@@ -37113,7 +37178,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>1235</v>
       </c>
@@ -37133,7 +37198,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>1231</v>
       </c>
@@ -37173,7 +37238,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>1223</v>
       </c>
@@ -37193,7 +37258,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>1219</v>
       </c>
@@ -37213,7 +37278,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>1215</v>
       </c>
@@ -37233,7 +37298,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>1211</v>
       </c>
@@ -37253,7 +37318,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>1207</v>
       </c>
@@ -37273,7 +37338,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>1203</v>
       </c>
@@ -37293,7 +37358,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>1198</v>
       </c>
@@ -37313,7 +37378,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
         <v>1194</v>
       </c>
@@ -37333,7 +37398,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
         <v>1190</v>
       </c>
@@ -37373,7 +37438,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
         <v>1182</v>
       </c>
@@ -37393,7 +37458,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>1178</v>
       </c>
@@ -37413,7 +37478,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>1174</v>
       </c>
@@ -37433,7 +37498,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
         <v>1170</v>
       </c>
@@ -37453,7 +37518,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>1166</v>
       </c>
@@ -37473,7 +37538,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
         <v>1162</v>
       </c>
@@ -37493,7 +37558,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
         <v>1157</v>
       </c>
@@ -37513,7 +37578,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>1153</v>
       </c>
@@ -37533,7 +37598,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
         <v>1149</v>
       </c>
@@ -37553,7 +37618,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
         <v>1145</v>
       </c>
@@ -37593,7 +37658,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="32" t="s">
         <v>1136</v>
       </c>
@@ -37613,7 +37678,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="32" t="s">
         <v>1132</v>
       </c>
@@ -37633,7 +37698,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="32" t="s">
         <v>1128</v>
       </c>
@@ -37653,7 +37718,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="32" t="s">
         <v>1124</v>
       </c>
@@ -37673,7 +37738,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
         <v>1120</v>
       </c>
@@ -37693,7 +37758,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
         <v>1116</v>
       </c>
@@ -37713,7 +37778,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
         <v>1112</v>
       </c>
@@ -37733,7 +37798,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="32" t="s">
         <v>1107</v>
       </c>
@@ -37753,7 +37818,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="32" t="s">
         <v>1102</v>
       </c>
@@ -37773,7 +37838,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="32" t="s">
         <v>1098</v>
       </c>
@@ -37793,7 +37858,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="32" t="s">
         <v>1094</v>
       </c>
@@ -37813,7 +37878,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="32" t="s">
         <v>1090</v>
       </c>
@@ -37833,7 +37898,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="32" t="s">
         <v>1085</v>
       </c>
@@ -37853,7 +37918,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="32" t="s">
         <v>1080</v>
       </c>
@@ -37873,7 +37938,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="32" t="s">
         <v>1075</v>
       </c>
@@ -37893,7 +37958,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="32" t="s">
         <v>1070</v>
       </c>
@@ -37913,7 +37978,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="32" t="s">
         <v>1065</v>
       </c>
@@ -37933,7 +37998,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="32" t="s">
         <v>1060</v>
       </c>
@@ -37953,7 +38018,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="32" t="s">
         <v>1055</v>
       </c>
@@ -37973,7 +38038,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="32" t="s">
         <v>1051</v>
       </c>
@@ -37993,7 +38058,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="32" t="s">
         <v>1046</v>
       </c>
@@ -38013,7 +38078,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="32" t="s">
         <v>1042</v>
       </c>
@@ -38033,7 +38098,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="32" t="s">
         <v>1038</v>
       </c>
@@ -38053,7 +38118,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="32" t="s">
         <v>1034</v>
       </c>
@@ -38073,7 +38138,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="32" t="s">
         <v>1029</v>
       </c>
@@ -38093,7 +38158,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="32" t="s">
         <v>1025</v>
       </c>
@@ -38113,7 +38178,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="32" t="s">
         <v>1020</v>
       </c>
@@ -38133,7 +38198,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="32" t="s">
         <v>1015</v>
       </c>
@@ -38173,7 +38238,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="32" t="s">
         <v>1006</v>
       </c>
@@ -38193,7 +38258,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="32" t="s">
         <v>1001</v>
       </c>
@@ -38213,7 +38278,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="32" t="s">
         <v>996</v>
       </c>
@@ -38233,7 +38298,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
         <v>991</v>
       </c>
@@ -38253,7 +38318,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="32" t="s">
         <v>986</v>
       </c>
@@ -38273,7 +38338,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="32" t="s">
         <v>980</v>
       </c>
@@ -38293,7 +38358,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="32" t="s">
         <v>975</v>
       </c>
@@ -38313,7 +38378,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="32" t="s">
         <v>969</v>
       </c>
@@ -38333,7 +38398,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="32" t="s">
         <v>964</v>
       </c>
@@ -38353,7 +38418,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="32" t="s">
         <v>958</v>
       </c>
@@ -38376,6 +38441,19 @@
     <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
+  <autoFilter ref="A7:F98">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter val="a*"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <customFilters and="1">
+        <customFilter operator="notEqual" val="m*"/>
+        <customFilter operator="notEqual" val="e*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -38385,13 +38463,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="B2:J103"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38453,7 +38531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
@@ -38540,7 +38618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -38569,7 +38647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -38685,7 +38763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
@@ -38772,7 +38850,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
@@ -38830,7 +38908,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
@@ -38888,7 +38966,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>85</v>
       </c>
@@ -38917,7 +38995,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>90</v>
       </c>
@@ -38975,7 +39053,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
@@ -39149,7 +39227,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>123</v>
       </c>
@@ -39178,7 +39256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>129</v>
       </c>
@@ -39294,7 +39372,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>149</v>
       </c>
@@ -39381,7 +39459,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>123</v>
       </c>
@@ -39468,7 +39546,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>178</v>
       </c>
@@ -39526,7 +39604,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>188</v>
       </c>
@@ -39555,7 +39633,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>193</v>
       </c>
@@ -39584,7 +39662,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>198</v>
       </c>
@@ -39613,7 +39691,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>203</v>
       </c>
@@ -39642,7 +39720,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>208</v>
       </c>
@@ -39729,7 +39807,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>224</v>
       </c>
@@ -39758,7 +39836,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>224</v>
       </c>
@@ -39787,7 +39865,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>208</v>
       </c>
@@ -39816,7 +39894,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>237</v>
       </c>
@@ -39845,7 +39923,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>242</v>
       </c>
@@ -39874,7 +39952,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>242</v>
       </c>
@@ -39903,7 +39981,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>251</v>
       </c>
@@ -39990,7 +40068,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>265</v>
       </c>
@@ -40019,7 +40097,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>265</v>
       </c>
@@ -40048,7 +40126,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>276</v>
       </c>
@@ -40077,7 +40155,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>281</v>
       </c>
@@ -40106,7 +40184,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>286</v>
       </c>
@@ -40164,7 +40242,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>296</v>
       </c>
@@ -40193,7 +40271,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>301</v>
       </c>
@@ -40222,7 +40300,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>306</v>
       </c>
@@ -40251,7 +40329,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>311</v>
       </c>
@@ -40280,7 +40358,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>311</v>
       </c>
@@ -40338,7 +40416,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>326</v>
       </c>
@@ -40367,7 +40445,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>331</v>
       </c>
@@ -40396,7 +40474,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>331</v>
       </c>
@@ -40454,7 +40532,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>345</v>
       </c>
@@ -40483,7 +40561,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>321</v>
       </c>
@@ -40541,7 +40619,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>360</v>
       </c>
@@ -40744,7 +40822,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>389</v>
       </c>
@@ -40773,7 +40851,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>394</v>
       </c>
@@ -40918,7 +40996,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>418</v>
       </c>
@@ -40976,7 +41054,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>426</v>
       </c>
@@ -41034,7 +41112,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>437</v>
       </c>
@@ -41063,7 +41141,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>432</v>
       </c>
@@ -41150,7 +41228,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>451</v>
       </c>
@@ -41267,6 +41345,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B6:J103">
+    <filterColumn colId="3">
+      <dynamicFilter type="aboveAverage" val="1697.2061855670104"/>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="J61" r:id="rId1" display="mailto:Pestrada@uni.edu.pe"/>
     <hyperlink ref="J67" r:id="rId2" display="mailto:galarcon63@hotmail.com"/>
@@ -41284,13 +41367,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A6:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -41326,7 +41409,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>1349</v>
       </c>
@@ -41346,7 +41429,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>1345</v>
       </c>
@@ -41366,7 +41449,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
         <v>1341</v>
       </c>
@@ -41386,7 +41469,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>1337</v>
       </c>
@@ -41406,7 +41489,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
         <v>1333</v>
       </c>
@@ -41426,7 +41509,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>1329</v>
       </c>
@@ -41446,7 +41529,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>1325</v>
       </c>
@@ -41466,7 +41549,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>1321</v>
       </c>
@@ -41486,7 +41569,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>1317</v>
       </c>
@@ -41506,7 +41589,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>1313</v>
       </c>
@@ -41526,7 +41609,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>1309</v>
       </c>
@@ -41546,7 +41629,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>1305</v>
       </c>
@@ -41566,7 +41649,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>1301</v>
       </c>
@@ -41586,7 +41669,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>1297</v>
       </c>
@@ -41606,7 +41689,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>1293</v>
       </c>
@@ -41626,7 +41709,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>1289</v>
       </c>
@@ -41646,7 +41729,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
         <v>1285</v>
       </c>
@@ -41666,7 +41749,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
         <v>1280</v>
       </c>
@@ -41686,7 +41769,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
         <v>1276</v>
       </c>
@@ -41706,7 +41789,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
         <v>1272</v>
       </c>
@@ -41726,7 +41809,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
         <v>1268</v>
       </c>
@@ -41746,7 +41829,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
         <v>1264</v>
       </c>
@@ -41766,7 +41849,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
         <v>1260</v>
       </c>
@@ -41786,7 +41869,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
         <v>1256</v>
       </c>
@@ -41806,7 +41889,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
         <v>1251</v>
       </c>
@@ -41826,7 +41909,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
         <v>1247</v>
       </c>
@@ -41846,7 +41929,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
         <v>1243</v>
       </c>
@@ -41866,7 +41949,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
         <v>1239</v>
       </c>
@@ -41886,7 +41969,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>1235</v>
       </c>
@@ -41906,7 +41989,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
         <v>1231</v>
       </c>
@@ -41926,7 +42009,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
         <v>1227</v>
       </c>
@@ -41946,7 +42029,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="s">
         <v>1223</v>
       </c>
@@ -41966,7 +42049,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="s">
         <v>1219</v>
       </c>
@@ -41986,7 +42069,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
         <v>1215</v>
       </c>
@@ -42026,7 +42109,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>1207</v>
       </c>
@@ -42046,7 +42129,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>1203</v>
       </c>
@@ -42066,7 +42149,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
         <v>1198</v>
       </c>
@@ -42086,7 +42169,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
         <v>1194</v>
       </c>
@@ -42106,7 +42189,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
         <v>1190</v>
       </c>
@@ -42126,7 +42209,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
         <v>1186</v>
       </c>
@@ -42146,7 +42229,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
         <v>1182</v>
       </c>
@@ -42166,7 +42249,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
         <v>1178</v>
       </c>
@@ -42186,7 +42269,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
         <v>1174</v>
       </c>
@@ -42206,7 +42289,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
         <v>1170</v>
       </c>
@@ -42246,7 +42329,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="35" t="s">
         <v>1162</v>
       </c>
@@ -42266,7 +42349,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
         <v>1157</v>
       </c>
@@ -42286,7 +42369,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="35" t="s">
         <v>1153</v>
       </c>
@@ -42306,7 +42389,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="35" t="s">
         <v>1149</v>
       </c>
@@ -42326,7 +42409,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="35" t="s">
         <v>1145</v>
       </c>
@@ -42346,7 +42429,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="35" t="s">
         <v>1140</v>
       </c>
@@ -42366,7 +42449,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="35" t="s">
         <v>1136</v>
       </c>
@@ -42386,7 +42469,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="35" t="s">
         <v>1132</v>
       </c>
@@ -42406,7 +42489,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="35" t="s">
         <v>1128</v>
       </c>
@@ -42426,7 +42509,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="35" t="s">
         <v>1124</v>
       </c>
@@ -42446,7 +42529,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36" t="s">
         <v>1120</v>
       </c>
@@ -42466,7 +42549,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>1116</v>
       </c>
@@ -42486,7 +42569,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="36" t="s">
         <v>1112</v>
       </c>
@@ -42506,7 +42589,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="35" t="s">
         <v>1107</v>
       </c>
@@ -42526,7 +42609,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="35" t="s">
         <v>1102</v>
       </c>
@@ -42546,7 +42629,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="35" t="s">
         <v>1098</v>
       </c>
@@ -42566,7 +42649,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="35" t="s">
         <v>1094</v>
       </c>
@@ -42586,7 +42669,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="35" t="s">
         <v>1090</v>
       </c>
@@ -42606,7 +42689,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="35" t="s">
         <v>1085</v>
       </c>
@@ -42626,7 +42709,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="35" t="s">
         <v>1080</v>
       </c>
@@ -42646,7 +42729,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="35" t="s">
         <v>1075</v>
       </c>
@@ -42666,7 +42749,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="35" t="s">
         <v>1070</v>
       </c>
@@ -42686,7 +42769,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="35" t="s">
         <v>1065</v>
       </c>
@@ -42706,7 +42789,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="35" t="s">
         <v>1060</v>
       </c>
@@ -42726,7 +42809,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="35" t="s">
         <v>1055</v>
       </c>
@@ -42746,7 +42829,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="35" t="s">
         <v>1051</v>
       </c>
@@ -42766,7 +42849,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="35" t="s">
         <v>1046</v>
       </c>
@@ -42786,7 +42869,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="35" t="s">
         <v>1042</v>
       </c>
@@ -42806,7 +42889,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="36" t="s">
         <v>1038</v>
       </c>
@@ -42826,7 +42909,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="36" t="s">
         <v>1034</v>
       </c>
@@ -42846,7 +42929,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="36" t="s">
         <v>1029</v>
       </c>
@@ -42866,7 +42949,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="35" t="s">
         <v>1025</v>
       </c>
@@ -42886,7 +42969,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="35" t="s">
         <v>1020</v>
       </c>
@@ -42906,7 +42989,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="35" t="s">
         <v>1015</v>
       </c>
@@ -42926,7 +43009,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="35" t="s">
         <v>1010</v>
       </c>
@@ -42946,7 +43029,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="35" t="s">
         <v>1006</v>
       </c>
@@ -42966,7 +43049,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="35" t="s">
         <v>1001</v>
       </c>
@@ -42986,7 +43069,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="35" t="s">
         <v>996</v>
       </c>
@@ -43006,7 +43089,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="35" t="s">
         <v>991</v>
       </c>
@@ -43026,7 +43109,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="35" t="s">
         <v>986</v>
       </c>
@@ -43046,7 +43129,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="35" t="s">
         <v>980</v>
       </c>
@@ -43066,7 +43149,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="36" t="s">
         <v>975</v>
       </c>
@@ -43086,7 +43169,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="36" t="s">
         <v>969</v>
       </c>
@@ -43106,7 +43189,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="36" t="s">
         <v>964</v>
       </c>
@@ -43126,7 +43209,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="35" t="s">
         <v>958</v>
       </c>
@@ -43148,6 +43231,16 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
+  <autoFilter ref="A6:F97">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Venezuela"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -43162,7 +43255,9 @@
   </sheetPr>
   <dimension ref="B1:J103"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A66" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>